<commit_message>
Modified Dependency Test case in 1PNotify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
   <si>
     <t>API</t>
   </si>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E13" workbookViewId="0">
-      <selection activeCell="L17" sqref="L2:L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -811,9 +811,6 @@
       <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
@@ -1039,7 +1036,7 @@
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Added New test case to 1PNOTIFY
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="152">
   <si>
     <t>API</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-484_posts.id)</t>
+  </si>
+  <si>
+    <t>OPQA-776</t>
+  </si>
+  <si>
+    <t>Verify that the admin can delete any post as a moderator</t>
+  </si>
+  <si>
+    <t>/administration/posts/(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=true</t>
   </si>
 </sst>
 </file>
@@ -842,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1565,350 +1577,358 @@
       </c>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="60">
-      <c r="A25" t="s">
+    <row r="25" spans="1:11" ht="30">
+      <c r="A25" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" ht="60">
+      <c r="A26" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>32</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="4" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>75</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="7" t="s">
+      <c r="K26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="30">
-      <c r="A26" t="s">
+    <row r="27" spans="1:11" ht="30">
+      <c r="A27" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>22</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>1</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>20</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>49</v>
       </c>
-      <c r="H26"/>
-      <c r="I26" t="s">
-        <v>78</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="60">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="H27"/>
       <c r="I27" t="s">
         <v>78</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" t="s">
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>18</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>22</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>1</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>19</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>23</v>
-      </c>
-      <c r="H28"/>
-      <c r="I28" t="s">
-        <v>87</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="60">
-      <c r="A29" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="H29"/>
       <c r="I29" t="s">
-        <v>78</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="60">
+      <c r="A30" s="7" t="s">
+        <v>125</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
       </c>
-      <c r="F30" t="s">
-        <v>31</v>
+      <c r="F30" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="H30"/>
       <c r="I30" t="s">
-        <v>62</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60">
-      <c r="A31" s="7" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>89</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31"/>
       <c r="I31" t="s">
         <v>62</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="60">
+      <c r="A32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" t="s">
+        <v>62</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K32" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>18</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>22</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>1</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>19</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>23</v>
-      </c>
-      <c r="H32"/>
-      <c r="I32" t="s">
-        <v>90</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="60">
-      <c r="A33" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="H33"/>
       <c r="I33" t="s">
         <v>90</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60">
+      <c r="A34" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>15</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="4"/>
-      <c r="J34" s="5" t="s">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="4"/>
+      <c r="J35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" ht="30">
-      <c r="A35" s="7" t="s">
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" ht="30">
+      <c r="A36" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>18</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>22</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E36" t="s">
         <v>1</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>19</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>23</v>
       </c>
-      <c r="H35"/>
-      <c r="I35" t="s">
+      <c r="H36"/>
+      <c r="I36" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36"/>
-      <c r="J36" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>56</v>
@@ -1917,13 +1937,34 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s">
         <v>14</v>
       </c>
       <c r="H37"/>
       <c r="J37" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38"/>
+      <c r="J38" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1932,10 +1973,10 @@
     <hyperlink ref="A4" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-874"/>
     <hyperlink ref="A7" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-208"/>
     <hyperlink ref="A10" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-206"/>
-    <hyperlink ref="A26" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-210"/>
-    <hyperlink ref="A28" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-209"/>
-    <hyperlink ref="A32" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-207"/>
-    <hyperlink ref="A35" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-213"/>
+    <hyperlink ref="A27" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-210"/>
+    <hyperlink ref="A29" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-209"/>
+    <hyperlink ref="A33" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-207"/>
+    <hyperlink ref="A36" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-213"/>
     <hyperlink ref="A2" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-875"/>
     <hyperlink ref="A3" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-876"/>
     <hyperlink ref="A15" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-215"/>

</xml_diff>

<commit_message>
Modified validations in 1PNotify Added Test cases in 1PRecommend
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -199,9 +199,6 @@
     <t>status=200||type=FRIENDS_FOLLOWED_OTHERS||issuer.truid=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||type=Appreciation||comment.issuer.truid=(SYS_USER1)||issuer.truid=(SYS_USER2)</t>
-  </si>
-  <si>
     <t>OPQA-874</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>OPQA-236_1</t>
   </si>
   <si>
-    <t>status=200||type[0]=WatchedDocumentComment||comments[0].data.id=(OPQA-236_1_comments.id)||type[0]=DocumentComment</t>
-  </si>
-  <si>
     <t>/appreciation/appreciate/Comment/(OPQA-236_1_comments.id)</t>
   </si>
   <si>
@@ -454,9 +448,6 @@
     <t>/comments/comment/(OPQA-385_1_comments.id)</t>
   </si>
   <si>
-    <t>status=200||type=Appreciation||comment.issuer.truid=(SYS_USER3)||issuer.truid=(SYS_USER1)</t>
-  </si>
-  <si>
     <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-484_posts.id)</t>
   </si>
   <si>
@@ -470,13 +461,22 @@
   </si>
   <si>
     <t>status=200||targetType=posts||targetId=(OPQA-360_id)||hasSucceeded=true</t>
+  </si>
+  <si>
+    <t>status=200||type[0]=WatchedDocumentComment||comments[0].data.id=(OPQA-236_1_comments.id)||type[1]=DocumentComment</t>
+  </si>
+  <si>
+    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER2)||comment.id=(OPQA-236_1_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER1)||comment.id=(OPQA-385_comments.id)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +488,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -534,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -560,6 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
@@ -916,7 +924,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>41</v>
@@ -943,7 +951,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>42</v>
@@ -967,13 +975,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -994,16 +1002,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -1013,7 +1021,7 @@
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>13</v>
@@ -1021,7 +1029,7 @@
     </row>
     <row r="6" spans="1:12" ht="60">
       <c r="A6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>45</v>
@@ -1040,10 +1048,10 @@
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>46</v>
@@ -1054,10 +1062,10 @@
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -1076,15 +1084,15 @@
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="60">
       <c r="A8" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>52</v>
@@ -1093,7 +1101,7 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1103,15 +1111,15 @@
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>40</v>
@@ -1136,7 +1144,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>43</v>
@@ -1158,7 +1166,7 @@
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
@@ -1166,16 +1174,16 @@
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>17</v>
@@ -1185,22 +1193,22 @@
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -1219,34 +1227,34 @@
       </c>
       <c r="H12"/>
       <c r="I12" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
         <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>13</v>
@@ -1254,10 +1262,10 @@
     </row>
     <row r="14" spans="1:12" ht="60">
       <c r="A14" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>32</v>
@@ -1269,17 +1277,17 @@
         <v>17</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>35</v>
@@ -1287,10 +1295,10 @@
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1309,18 +1317,18 @@
       </c>
       <c r="H15"/>
       <c r="I15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -1339,24 +1347,24 @@
       </c>
       <c r="H16"/>
       <c r="I16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60">
       <c r="A17" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>17</v>
@@ -1369,19 +1377,19 @@
         <v>36</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1393,38 +1401,38 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
       </c>
       <c r="H18"/>
       <c r="J18" s="5" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>13</v>
@@ -1432,27 +1440,27 @@
     </row>
     <row r="20" spans="1:11" ht="60">
       <c r="A20" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>13</v>
@@ -1461,16 +1469,16 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>1</v>
@@ -1485,15 +1493,15 @@
         <v>13</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="60">
       <c r="A22" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>32</v>
@@ -1509,13 +1517,13 @@
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>35</v>
@@ -1523,10 +1531,10 @@
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -1545,21 +1553,21 @@
       </c>
       <c r="H23"/>
       <c r="J23" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60">
       <c r="A24" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>14</v>
@@ -1570,7 +1578,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>13</v>
@@ -1579,16 +1587,16 @@
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>14</v>
@@ -1599,16 +1607,16 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" ht="60">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>45</v>
@@ -1627,10 +1635,10 @@
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>46</v>
@@ -1640,8 +1648,8 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
-      <c r="A27" t="s">
-        <v>86</v>
+      <c r="A27" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>48</v>
@@ -1663,15 +1671,15 @@
       </c>
       <c r="H27"/>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="60">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>50</v>
@@ -1680,7 +1688,7 @@
         <v>32</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
         <v>17</v>
@@ -1692,15 +1700,15 @@
         <v>36</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="30">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>51</v>
@@ -1722,15 +1730,15 @@
       </c>
       <c r="H29"/>
       <c r="I29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>61</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60">
       <c r="A30" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>52</v>
@@ -1739,7 +1747,7 @@
         <v>32</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -1749,15 +1757,15 @@
       </c>
       <c r="H30"/>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>53</v>
@@ -1766,7 +1774,7 @@
         <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
@@ -1776,7 +1784,7 @@
       </c>
       <c r="H31"/>
       <c r="I31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J31" s="5" t="s">
         <v>13</v>
@@ -1784,7 +1792,7 @@
     </row>
     <row r="32" spans="1:11" ht="60">
       <c r="A32" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>55</v>
@@ -1803,10 +1811,10 @@
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>54</v>
@@ -1817,7 +1825,7 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>47</v>
@@ -1839,15 +1847,15 @@
       </c>
       <c r="H33"/>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
       <c r="A34" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>52</v>
@@ -1856,7 +1864,7 @@
         <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
@@ -1866,15 +1874,15 @@
       </c>
       <c r="H34"/>
       <c r="I34" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>58</v>
@@ -1898,7 +1906,7 @@
     </row>
     <row r="36" spans="1:11" ht="30">
       <c r="A36" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>59</v>
@@ -1920,7 +1928,7 @@
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J36" s="5" t="s">
         <v>60</v>
@@ -1928,7 +1936,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>56</v>
@@ -1949,7 +1957,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Fixed failing test case in 1PNOTIFY
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="170">
   <si>
     <t>API</t>
   </si>
@@ -542,6 +542,9 @@
   </si>
   <si>
     <t>Verify that user is able to update watch list from  private to public</t>
+  </si>
+  <si>
+    <t>?size=3</t>
   </si>
 </sst>
 </file>
@@ -942,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L40"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2024,7 +2027,7 @@
         <v>45</v>
       </c>
       <c r="G36" t="s">
-        <v>46</v>
+        <v>169</v>
       </c>
       <c r="H36"/>
       <c r="I36" t="s">

</xml_diff>

<commit_message>
Fixed failing test case in notify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="169">
   <si>
     <t>API</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
-  </si>
-  <si>
-    <t>status=200||type=MyDocumentComment||comments.data.id=(OPQA-385_1_comments.id)||comments.data.issuer.truid=(SYS_USER3)</t>
   </si>
   <si>
     <t>status=200||id=(OPQA-385_1_comments.id)</t>
@@ -945,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="H35" workbookViewId="0">
+      <selection activeCell="L40" sqref="L2:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1194,7 +1191,7 @@
     </row>
     <row r="9" spans="1:12" ht="105">
       <c r="A9" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>16</v>
@@ -1225,10 +1222,10 @@
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1247,37 +1244,37 @@
       </c>
       <c r="H10"/>
       <c r="I10" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="75">
       <c r="A11" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>12</v>
@@ -1286,29 +1283,29 @@
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>12</v>
@@ -1317,10 +1314,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1339,15 +1336,15 @@
       </c>
       <c r="H13"/>
       <c r="I13" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="75">
       <c r="A14" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>100</v>
@@ -1356,19 +1353,19 @@
         <v>17</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>12</v>
@@ -1425,7 +1422,7 @@
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16"/>
       <c r="I16" s="8" t="s">
@@ -1493,7 +1490,7 @@
         <v>67</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K18" s="8"/>
     </row>
@@ -1517,14 +1514,14 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
         <v>84</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="60">
@@ -1551,7 +1548,7 @@
         <v>41</v>
       </c>
       <c r="I20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>85</v>
@@ -1705,7 +1702,7 @@
         <v>99</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60">
@@ -1737,7 +1734,7 @@
     </row>
     <row r="27" spans="1:11" ht="75">
       <c r="A27" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>101</v>
@@ -1746,19 +1743,19 @@
         <v>17</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" t="s">
         <v>148</v>
-      </c>
-      <c r="I27" t="s">
-        <v>149</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>12</v>
@@ -1788,7 +1785,7 @@
         <v>105</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>124</v>
@@ -1824,7 +1821,7 @@
         <v>103</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30">
@@ -1854,7 +1851,7 @@
         <v>103</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="60">
@@ -1944,7 +1941,7 @@
         <v>119</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="60">
@@ -2027,14 +2024,14 @@
         <v>45</v>
       </c>
       <c r="G36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
         <v>123</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>125</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="60">
@@ -2048,7 +2045,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
         <v>50</v>
@@ -2061,15 +2058,15 @@
         <v>123</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="C38" t="s">
         <v>54</v>
@@ -2082,15 +2079,15 @@
       </c>
       <c r="H38"/>
       <c r="J38" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
         <v>54</v>
@@ -2103,21 +2100,21 @@
       </c>
       <c r="H39"/>
       <c r="J39" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="30">
       <c r="A40" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40" s="10" t="s">
         <v>50</v>
@@ -2131,7 +2128,7 @@
         <v>67</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K40" s="8"/>
     </row>

</xml_diff>

<commit_message>
Changed test cases in Notify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H35" workbookViewId="0">
-      <selection activeCell="L40" sqref="L2:L40"/>
+    <sheetView tabSelected="1" topLeftCell="H37" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1514,7 +1514,7 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
@@ -1695,7 +1695,7 @@
         <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
@@ -1934,7 +1934,7 @@
         <v>45</v>
       </c>
       <c r="G33" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="H33"/>
       <c r="I33" t="s">

</xml_diff>

<commit_message>
Modified test cases in notify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="171">
   <si>
     <t>API</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>?size=3</t>
+  </si>
+  <si>
+    <t>OPQA-218</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification if someone likes his comment on a post</t>
   </si>
 </sst>
 </file>
@@ -942,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L40"/>
     </sheetView>
   </sheetViews>
@@ -1514,7 +1520,7 @@
         <v>45</v>
       </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="H19"/>
       <c r="I19" t="s">
@@ -1695,7 +1701,7 @@
         <v>45</v>
       </c>
       <c r="G25" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="H25"/>
       <c r="I25" t="s">
@@ -1916,10 +1922,10 @@
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>169</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1934,7 +1940,7 @@
         <v>45</v>
       </c>
       <c r="G33" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="H33"/>
       <c r="I33" t="s">

</xml_diff>

<commit_message>
Fixed failing test cases
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L40"/>
+    <sheetView tabSelected="1" topLeftCell="H35" workbookViewId="0">
+      <selection activeCell="L40" sqref="L2:L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1131,7 +1131,7 @@
         <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
@@ -1185,7 +1185,7 @@
         <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
@@ -1246,7 +1246,7 @@
         <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H10"/>
       <c r="I10" s="5" t="s">
@@ -1338,7 +1338,7 @@
         <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H13"/>
       <c r="I13" s="5" t="s">

</xml_diff>

<commit_message>
Added Test cases in 1PNotify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="177">
   <si>
     <t>API</t>
   </si>
@@ -548,6 +548,24 @@
   </si>
   <si>
     <t>Verify that user receives a notification if someone likes his comment on a post</t>
+  </si>
+  <si>
+    <t>OPQA-1395</t>
+  </si>
+  <si>
+    <t>OPQA-207_1</t>
+  </si>
+  <si>
+    <t>Verify that all users receive notification when other user published a post .</t>
+  </si>
+  <si>
+    <t>Verify that user should receive notification when other user published a comment on an article.</t>
+  </si>
+  <si>
+    <t>X-1P-User=5cb7317e-6856-4c2a-bb0e-5302eeec03f1</t>
+  </si>
+  <si>
+    <t>OPQA-1397</t>
   </si>
 </sst>
 </file>
@@ -946,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H35" workbookViewId="0">
-      <selection activeCell="L40" sqref="L2:L40"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -959,7 +977,7 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1377,7 +1395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="60">
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
         <v>67</v>
       </c>
@@ -1438,40 +1456,39 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="60">
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>38</v>
+        <v>173</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="11" t="s">
-        <v>77</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17"/>
       <c r="I17" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="60">
+      <c r="J17" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30">
       <c r="A18" s="8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>78</v>
@@ -1485,8 +1502,8 @@
       <c r="E18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>66</v>
+      <c r="F18" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11" t="s">
@@ -1496,109 +1513,110 @@
         <v>67</v>
       </c>
       <c r="J18" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" ht="30">
+      <c r="A19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="30">
-      <c r="A19" s="5" t="s">
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>45</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>33</v>
       </c>
-      <c r="H19"/>
-      <c r="I19" t="s">
+      <c r="H20"/>
+      <c r="I20" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="60">
-      <c r="A20" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" t="s">
-        <v>150</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H21"/>
+        <v>39</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>90</v>
+        <v>150</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" s="8" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
         <v>30</v>
@@ -1610,7 +1628,7 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
         <v>46</v>
@@ -1620,312 +1638,312 @@
         <v>37</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="60">
-      <c r="A23" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>77</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23"/>
       <c r="I23" t="s">
         <v>37</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="60">
-      <c r="A24" t="s">
-        <v>95</v>
+      <c r="J23" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>93</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>77</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24"/>
       <c r="I24" t="s">
         <v>37</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>96</v>
+      <c r="J24" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" t="s">
-        <v>45</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25"/>
+        <v>13</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="I25" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="60">
-      <c r="A26" s="8" t="s">
-        <v>47</v>
+        <v>37</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="30">
+      <c r="A26" t="s">
+        <v>95</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26"/>
+        <v>66</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="I26" t="s">
         <v>37</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="75">
-      <c r="A27" s="5" t="s">
-        <v>151</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30">
+      <c r="A27" t="s">
+        <v>97</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>147</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27"/>
       <c r="I27" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="60">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="8" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>13</v>
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="H28"/>
       <c r="I28" t="s">
-        <v>152</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
-      <c r="A29" s="8" t="s">
-        <v>109</v>
+        <v>37</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75">
+      <c r="A29" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29"/>
-      <c r="I29" s="8" t="s">
-        <v>103</v>
+        <v>130</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29" t="s">
+        <v>148</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>133</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30" t="s">
+        <v>152</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30">
+      <c r="A31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>25</v>
       </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="s">
         <v>46</v>
       </c>
-      <c r="H30"/>
-      <c r="I30" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="60">
-      <c r="A31" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="H31"/>
       <c r="I31" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J31" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="K31" s="8"/>
-    </row>
-    <row r="32" spans="1:11" ht="60">
+      <c r="J31" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>38</v>
+        <v>112</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>77</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32"/>
       <c r="I32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J32" s="9" t="s">
-        <v>118</v>
+      <c r="J32" s="5" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
-      <c r="A33" t="s">
-        <v>169</v>
+      <c r="A33" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>170</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1937,85 +1955,85 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H33"/>
-      <c r="I33" t="s">
-        <v>119</v>
+      <c r="I33" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="60">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" t="s">
-        <v>50</v>
+        <v>114</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34"/>
+        <v>40</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="I34" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="60">
+      <c r="J34" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I35" t="s">
-        <v>67</v>
+      <c r="H35" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K35" s="10" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30">
-      <c r="A36" s="5" t="s">
-        <v>107</v>
+      <c r="A36" t="s">
+        <v>169</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>108</v>
+        <v>170</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -2030,17 +2048,17 @@
         <v>45</v>
       </c>
       <c r="G36" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="60">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30">
       <c r="A37" s="8" t="s">
         <v>121</v>
       </c>
@@ -2051,92 +2069,182 @@
         <v>38</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
         <v>50</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="30">
+      <c r="A38" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="B38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" t="s">
+        <v>67</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30">
+      <c r="A39" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39" t="s">
+        <v>123</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30">
+      <c r="A40" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40"/>
+      <c r="I40" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E41" t="s">
         <v>50</v>
       </c>
-      <c r="H38"/>
-      <c r="J38" s="5" t="s">
+      <c r="H41"/>
+      <c r="J41" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D42" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E42" t="s">
         <v>50</v>
       </c>
-      <c r="H39"/>
-      <c r="J39" s="5" t="s">
+      <c r="H42"/>
+      <c r="J42" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30">
-      <c r="A40" s="12" t="s">
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
         <v>138</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D43" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F43" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8" t="s">
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="J40" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="K40" s="8"/>
+      <c r="K43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed Failing test case
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
   <si>
     <t>API</t>
   </si>
@@ -159,9 +159,6 @@
     <t>X-1P-User=(SYS_USER2)</t>
   </si>
   <si>
-    <t>?size=1</t>
-  </si>
-  <si>
     <t>OPQA-286</t>
   </si>
   <si>
@@ -445,9 +442,6 @@
   </si>
   <si>
     <t>status=200||userId=(SYS_USER2)||id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>?size=2</t>
   </si>
   <si>
     <t>OPQA-312</t>
@@ -539,9 +533,6 @@
   </si>
   <si>
     <t>Verify that user is able to update watch list from  private to public</t>
-  </si>
-  <si>
-    <t>?size=3</t>
   </si>
   <si>
     <t>OPQA-218</t>
@@ -966,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L43"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1106,16 +1097,16 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -1125,16 +1116,16 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -1153,24 +1144,24 @@
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
@@ -1179,16 +1170,16 @@
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
       <c r="J7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1207,15 +1198,15 @@
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="105">
       <c r="A9" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>16</v>
@@ -1230,7 +1221,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="4" t="s">
@@ -1246,10 +1237,10 @@
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1268,37 +1259,37 @@
       </c>
       <c r="H10"/>
       <c r="I10" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="75">
       <c r="A11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>12</v>
@@ -1307,29 +1298,29 @@
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>12</v>
@@ -1338,10 +1329,10 @@
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1360,36 +1351,36 @@
       </c>
       <c r="H13"/>
       <c r="I13" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="75">
       <c r="A14" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>12</v>
@@ -1397,16 +1388,16 @@
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>13</v>
@@ -1416,22 +1407,22 @@
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -1446,22 +1437,22 @@
         <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="H16"/>
       <c r="I16" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -1473,31 +1464,31 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
       </c>
       <c r="H17"/>
       <c r="I17" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>13</v>
@@ -1507,53 +1498,53 @@
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C20" t="s">
         <v>30</v>
@@ -1572,10 +1563,10 @@
       </c>
       <c r="H20"/>
       <c r="I20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30">
@@ -1583,7 +1574,7 @@
         <v>37</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
@@ -1602,10 +1593,10 @@
         <v>41</v>
       </c>
       <c r="I21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>42</v>
@@ -1628,25 +1619,25 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G22" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H22"/>
       <c r="I22" t="s">
         <v>37</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1661,22 +1652,22 @@
         <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
         <v>37</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
         <v>30</v>
@@ -1688,7 +1679,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
@@ -1698,21 +1689,21 @@
         <v>37</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1721,50 +1712,50 @@
         <v>40</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
         <v>37</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
         <v>37</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="C27" t="s">
         <v>30</v>
@@ -1783,27 +1774,27 @@
       </c>
       <c r="H27"/>
       <c r="I27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30">
       <c r="A28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
         <v>49</v>
-      </c>
-      <c r="E28" t="s">
-        <v>50</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>14</v>
@@ -1813,33 +1804,33 @@
         <v>37</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="75">
       <c r="A29" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>12</v>
@@ -1847,10 +1838,10 @@
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>38</v>
@@ -1866,13 +1857,13 @@
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>42</v>
@@ -1880,10 +1871,10 @@
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>
@@ -1895,25 +1886,25 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H31"/>
       <c r="I31" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
@@ -1928,22 +1919,22 @@
         <v>32</v>
       </c>
       <c r="G32" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H32"/>
       <c r="I32" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -1955,31 +1946,31 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G33" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="H33"/>
       <c r="I33" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>13</v>
@@ -1989,51 +1980,51 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30">
       <c r="A36" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
         <v>30</v>
@@ -2052,45 +2043,45 @@
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30">
       <c r="A37" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30">
       <c r="A38" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>38</v>
@@ -2102,17 +2093,17 @@
         <v>13</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I38" t="s">
+        <v>66</v>
+      </c>
+      <c r="J38" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="I38" t="s">
-        <v>67</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="K38" s="10" t="s">
         <v>42</v>
@@ -2120,10 +2111,10 @@
     </row>
     <row r="39" spans="1:11" ht="30">
       <c r="A39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="C39" t="s">
         <v>30</v>
@@ -2138,11 +2129,11 @@
         <v>45</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>33</v>
       </c>
       <c r="H39"/>
       <c r="I39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J39" s="5" t="s">
         <v>12</v>
@@ -2150,88 +2141,88 @@
     </row>
     <row r="40" spans="1:11" ht="30">
       <c r="A40" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H40"/>
       <c r="I40" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>127</v>
-      </c>
       <c r="C41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="E41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H41"/>
       <c r="J41" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H42"/>
       <c r="J42" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
+        <v>137</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>45</v>
@@ -2239,10 +2230,10 @@
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K43" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added Test cases into 1PNOTIFY
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="195">
   <si>
     <t>API</t>
   </si>
@@ -544,19 +544,86 @@
     <t>OPQA-1395</t>
   </si>
   <si>
-    <t>OPQA-207_1</t>
-  </si>
-  <si>
     <t>Verify that all users receive notification when other user published a post .</t>
   </si>
   <si>
     <t>Verify that user should receive notification when other user published a comment on an article.</t>
   </si>
   <si>
-    <t>X-1P-User=5cb7317e-6856-4c2a-bb0e-5302eeec03f1</t>
-  </si>
-  <si>
     <t>OPQA-1397</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER4)</t>
+  </si>
+  <si>
+    <t>OPQA-898</t>
+  </si>
+  <si>
+    <t>Verify that to get patent id  for adding document in to users watch list</t>
+  </si>
+  <si>
+    <t>/patents/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;fields=sortdate&amp;sort=sortdate:desc&amp;size=1</t>
+  </si>
+  <si>
+    <t>Verify that user able to add patent in to his watchlist for notification test</t>
+  </si>
+  <si>
+    <t>/containers/(OPQA-312_containerId)/items/patents::(OPQA-898_hits.hits._id)?itemType=patents</t>
+  </si>
+  <si>
+    <t>{
+"containerId":"(OPQA-312_containerId)"
+"itemId":"patents::(OPQA-898_hits.hits._id)"
+"itemType":"patents"
+}</t>
+  </si>
+  <si>
+    <t>OPQA-898||OPQA-312</t>
+  </si>
+  <si>
+    <t>OPQA-310_2</t>
+  </si>
+  <si>
+    <t>Verify that user2 create comment in user3 watching patent</t>
+  </si>
+  <si>
+    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.hits._id)","content":"Notification Test"}</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone comments on a patent contained in his watchlist</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification when someone he is following comments on a patent</t>
+  </si>
+  <si>
+    <t>Verify that user should receive notification when other user published a comment on a patent.</t>
+  </si>
+  <si>
+    <t>OPQA-1420</t>
+  </si>
+  <si>
+    <t>OPQA-1421</t>
+  </si>
+  <si>
+    <t>OPQA-286_2</t>
+  </si>
+  <si>
+    <t>OPQA-1431</t>
+  </si>
+  <si>
+    <t>/comments/comment/(OPQA-1431_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||id=(OPQA-1431_comments.id)</t>
+  </si>
+  <si>
+    <t>OPQA-1432</t>
+  </si>
+  <si>
+    <t>OPQA-1433</t>
   </si>
 </sst>
 </file>
@@ -632,7 +699,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -659,7 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -955,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1096,220 +1162,216 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5"/>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="5" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6"/>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="J7" s="5" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="J8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" s="8" t="s">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="H8"/>
-      <c r="I8" t="s">
+      <c r="H9"/>
+      <c r="I9" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="105">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:12" ht="105">
+      <c r="A10" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="4" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="5" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="H10"/>
-      <c r="I10" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="75">
-      <c r="A11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="4" t="s">
-        <v>153</v>
-      </c>
+      <c r="H11"/>
       <c r="I11" s="5" t="s">
         <v>141</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1"/>
+        <v>151</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1317,7 +1379,7 @@
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>141</v>
@@ -1327,132 +1389,133 @@
       </c>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="30">
-      <c r="A13" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>158</v>
+    <row r="13" spans="1:12" ht="75">
+      <c r="A13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13"/>
+        <v>156</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="I13" s="5" t="s">
         <v>141</v>
       </c>
       <c r="J13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="75">
-      <c r="A14" s="5" t="s">
+    <row r="15" spans="1:12" ht="75">
+      <c r="A15" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>129</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>147</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30">
-      <c r="A15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B17" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16"/>
-      <c r="I16" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -1464,7 +1527,7 @@
         <v>25</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>33</v>
@@ -1477,40 +1540,39 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30">
+    <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>169</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="11" t="s">
-        <v>76</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18"/>
       <c r="I18" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="J18" s="5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>77</v>
@@ -1524,8 +1586,8 @@
       <c r="E19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>65</v>
+      <c r="F19" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="11" t="s">
@@ -1535,109 +1597,110 @@
         <v>66</v>
       </c>
       <c r="J19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" ht="30">
-      <c r="A20" s="5" t="s">
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>25</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>45</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>33</v>
       </c>
-      <c r="H20"/>
-      <c r="I20" t="s">
+      <c r="H21"/>
+      <c r="I21" t="s">
         <v>83</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" t="s">
-        <v>148</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F22" t="s">
-        <v>85</v>
-      </c>
-      <c r="G22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22"/>
+        <v>39</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I22" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>89</v>
+        <v>148</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="8" t="s">
-        <v>86</v>
+        <v>43</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>87</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>30</v>
@@ -1649,7 +1712,7 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
         <v>33</v>
@@ -1659,15 +1722,15 @@
         <v>37</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="12" t="s">
-        <v>169</v>
+      <c r="A24" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>171</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
         <v>30</v>
@@ -1679,7 +1742,7 @@
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="G24" t="s">
         <v>33</v>
@@ -1693,37 +1756,38 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
-      <c r="A25" t="s">
-        <v>90</v>
+      <c r="A25" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25"/>
       <c r="I25" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>93</v>
+      <c r="J25" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>91</v>
@@ -1738,7 +1802,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>76</v>
@@ -1747,164 +1811,163 @@
         <v>37</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
+      <c r="A28" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>25</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>45</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>33</v>
-      </c>
-      <c r="H27"/>
-      <c r="I27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>14</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="s">
+        <v>98</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29"/>
+      <c r="I29" t="s">
         <v>37</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="75">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:11" ht="75">
+      <c r="A30" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D30" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F30" t="s">
         <v>129</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>146</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
-      <c r="A30" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I30" t="s">
-        <v>150</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
+        <v>103</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" t="s">
-        <v>33</v>
-      </c>
-      <c r="H31"/>
-      <c r="I31" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>132</v>
+        <v>39</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I31" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K31" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
@@ -1916,7 +1979,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
@@ -1926,12 +1989,12 @@
         <v>102</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="8" t="s">
-        <v>173</v>
+        <v>110</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>111</v>
@@ -1946,7 +2009,7 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>172</v>
+        <v>32</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
@@ -1961,38 +2024,37 @@
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>38</v>
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
+        <v>30</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G34" s="8"/>
-      <c r="H34" s="9" t="s">
-        <v>76</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>172</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34"/>
       <c r="I34" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="K34" s="8"/>
+      <c r="J34" s="5" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>115</v>
@@ -2003,239 +2065,449 @@
       <c r="D35" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H35" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9" t="s">
         <v>76</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>102</v>
       </c>
       <c r="J35" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:11" ht="30">
+      <c r="A36" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="30">
-      <c r="A36" t="s">
+    <row r="37" spans="1:11" ht="30">
+      <c r="A37" t="s">
         <v>166</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>25</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>45</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G37" t="s">
         <v>33</v>
       </c>
-      <c r="H36"/>
-      <c r="I36" t="s">
+      <c r="H37"/>
+      <c r="I37" t="s">
         <v>118</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J37" s="5" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="30">
-      <c r="A37" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37"/>
-      <c r="I37" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="30">
       <c r="A38" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30">
+      <c r="A39" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E39" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9" t="s">
+      <c r="G39" s="8"/>
+      <c r="H39" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I39" t="s">
         <v>66</v>
       </c>
-      <c r="J38" s="9" t="s">
+      <c r="J39" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="K38" s="10" t="s">
+      <c r="K39" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="30">
-      <c r="A39" s="5" t="s">
+    <row r="40" spans="1:11" ht="30">
+      <c r="A40" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>25</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>45</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G40" t="s">
         <v>33</v>
       </c>
-      <c r="H39"/>
-      <c r="I39" t="s">
+      <c r="H40"/>
+      <c r="I40" t="s">
         <v>122</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="30">
-      <c r="A40" s="8" t="s">
+    <row r="41" spans="1:11" ht="30">
+      <c r="A41" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>38</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="E40" t="s">
-        <v>49</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H40"/>
-      <c r="I40" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="E41" t="s">
         <v>49</v>
       </c>
+      <c r="F41" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="H41"/>
-      <c r="J41" s="5" t="s">
+      <c r="I41" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="75">
+      <c r="A42" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I42" t="s">
+        <v>180</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="30">
+      <c r="A43" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="8"/>
+      <c r="H43" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="I43" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="30">
+      <c r="A44" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" t="s">
+        <v>33</v>
+      </c>
+      <c r="H44"/>
+      <c r="I44" t="s">
+        <v>190</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="30">
+      <c r="A45" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" t="s">
+        <v>32</v>
+      </c>
+      <c r="G45" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45"/>
+      <c r="I45" t="s">
+        <v>190</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="30">
+      <c r="A46" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
+        <v>172</v>
+      </c>
+      <c r="G46" t="s">
+        <v>33</v>
+      </c>
+      <c r="H46"/>
+      <c r="I46" t="s">
+        <v>190</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="30">
+      <c r="A47" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47"/>
+      <c r="I47" t="s">
+        <v>190</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="H48"/>
+      <c r="J48" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C49" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D49" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E49" t="s">
         <v>49</v>
       </c>
-      <c r="H42"/>
-      <c r="J42" s="5" t="s">
+      <c r="H49"/>
+      <c r="J49" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
         <v>137</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E50" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F50" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8" t="s">
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="J50" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="K43" s="8"/>
+      <c r="K50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixing failing test cases in notifications
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="197">
   <si>
     <t>API</t>
   </si>
@@ -624,6 +624,12 @@
   </si>
   <si>
     <t>OPQA-1433</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-898_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-898_hits.hits._id)</t>
   </si>
 </sst>
 </file>
@@ -2348,7 +2354,7 @@
         <v>190</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>89</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="30">
@@ -2378,7 +2384,7 @@
         <v>190</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>88</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="30">
@@ -2408,7 +2414,7 @@
         <v>190</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>88</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="30">

</xml_diff>

<commit_message>
Fixed Failing tests in notify
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="191">
   <si>
     <t>API</t>
   </si>
@@ -336,9 +336,6 @@
     <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Notification Test"}</t>
   </si>
   <si>
-    <t>status=200||comments.userId=(SYS_USER3)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
-  </si>
-  <si>
     <t>OPQA-215</t>
   </si>
   <si>
@@ -387,15 +384,6 @@
     <t>status=200||id=(OPQA-385_comments.id)</t>
   </si>
   <si>
-    <t>OPQA-385_1</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
-  </si>
-  <si>
-    <t>status=200||id=(OPQA-385_1_comments.id)</t>
-  </si>
-  <si>
     <t>OPQA-461</t>
   </si>
   <si>
@@ -414,12 +402,6 @@
     <t>status=200||hasAppreciated=UP||targetType=posts||appreciateCount=2||targetId=(OPQA-360_id)</t>
   </si>
   <si>
-    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-360_id)</t>
-  </si>
-  <si>
     <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||comment.id=(OPQA-385_comments.id)||comment.text=Notification Test</t>
   </si>
   <si>
@@ -427,9 +409,6 @@
   </si>
   <si>
     <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||publication.id=(OPQA-360_id)||publication.title=Creating Post For API Notification Testing</t>
-  </si>
-  <si>
-    <t>/comments/comment/(OPQA-385_1_comments.id)</t>
   </si>
   <si>
     <t>OPQA-1076</t>
@@ -479,9 +458,6 @@
     <t>OPQA-310_1</t>
   </si>
   <si>
-    <t>OPQA-360||OPQA-310_1</t>
-  </si>
-  <si>
     <t>status=200||type=PUBLIC_WATCHLIST||issuer.truid=(SYS_USER3)||publication.id=(OPQA-312_containerId)||publication.action=CREATE_WATCHLIST</t>
   </si>
   <si>
@@ -547,12 +523,6 @@
     <t>Verify that all users receive notification when other user published a post .</t>
   </si>
   <si>
-    <t>Verify that user should receive notification when other user published a comment on an article.</t>
-  </si>
-  <si>
-    <t>OPQA-1397</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER4)</t>
   </si>
   <si>
@@ -599,15 +569,6 @@
     <t>Verify that user receives a notification when someone he is following comments on a patent</t>
   </si>
   <si>
-    <t>Verify that user should receive notification when other user published a comment on a patent.</t>
-  </si>
-  <si>
-    <t>OPQA-1420</t>
-  </si>
-  <si>
-    <t>OPQA-1421</t>
-  </si>
-  <si>
     <t>OPQA-286_2</t>
   </si>
   <si>
@@ -630,6 +591,27 @@
   </si>
   <si>
     <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-898_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>OPQA-236||OPQA-310</t>
+  </si>
+  <si>
+    <t>OPQA-385||OPQA-310_1</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER4)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER4)||comments.data.text=Notification Test||publication.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER4)||comment.text=Notification Test||publication.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>OPQA-1431||OPQA-310_2</t>
   </si>
 </sst>
 </file>
@@ -705,7 +687,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -732,6 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1027,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L50"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1043,7 +1026,7 @@
     <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="93.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1169,22 +1152,22 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="1" t="s">
@@ -1305,7 +1288,7 @@
     </row>
     <row r="10" spans="1:12" ht="105">
       <c r="A10" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
@@ -1336,10 +1319,10 @@
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1358,37 +1341,37 @@
       </c>
       <c r="H11"/>
       <c r="I11" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>12</v>
@@ -1397,29 +1380,29 @@
     </row>
     <row r="13" spans="1:12" ht="75">
       <c r="A13" s="4" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>65</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="4" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>12</v>
@@ -1428,10 +1411,10 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -1450,15 +1433,15 @@
       </c>
       <c r="H14"/>
       <c r="I14" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="75">
       <c r="A15" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>99</v>
@@ -1467,19 +1450,19 @@
         <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>12</v>
@@ -1548,10 +1531,10 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1634,7 +1617,7 @@
         <v>66</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="K20" s="8"/>
     </row>
@@ -1665,7 +1648,7 @@
         <v>83</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
@@ -1692,7 +1675,7 @@
         <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>84</v>
@@ -1725,7 +1708,7 @@
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>37</v>
+        <v>184</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>89</v>
@@ -1762,38 +1745,37 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
-      <c r="A25" s="8" t="s">
-        <v>187</v>
+      <c r="A25" t="s">
+        <v>90</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>170</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" t="s">
-        <v>172</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25"/>
+        <v>13</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="I25" t="s">
         <v>37</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>88</v>
+      <c r="J25" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>91</v>
@@ -1808,7 +1790,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>76</v>
@@ -1817,163 +1799,164 @@
         <v>37</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27"/>
+      <c r="I27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
+      <c r="A28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" t="s">
-        <v>30</v>
-      </c>
       <c r="D28" s="6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" t="s">
-        <v>45</v>
-      </c>
-      <c r="G28" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="s">
-        <v>98</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
-      <c r="A29" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75">
+      <c r="A29" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>125</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I29" t="s">
+        <v>139</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29"/>
-      <c r="I29" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="75">
-      <c r="A30" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F30" t="s">
-        <v>129</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>145</v>
+      <c r="F30" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="I30" t="s">
-        <v>146</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>12</v>
+        <v>66</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="8" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>38</v>
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I31" t="s">
-        <v>150</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K31" s="10" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
@@ -1985,7 +1968,7 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="G32" t="s">
         <v>33</v>
@@ -1995,15 +1978,15 @@
         <v>102</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
-      <c r="A33" s="8" t="s">
-        <v>110</v>
+      <c r="A33" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
@@ -2015,205 +1998,204 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="G33" t="s">
         <v>33</v>
       </c>
       <c r="H33"/>
-      <c r="I33" s="8" t="s">
+      <c r="I33" t="s">
         <v>102</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>131</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" t="s">
-        <v>30</v>
+        <v>114</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" t="s">
-        <v>172</v>
-      </c>
-      <c r="G34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34"/>
+        <v>112</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G34" s="8"/>
+      <c r="H34" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="I34" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="5" t="s">
-        <v>131</v>
-      </c>
+      <c r="J34" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E35" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35" s="5" t="s">
         <v>76</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>102</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="K35" s="8"/>
+        <v>116</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="30">
-      <c r="A36" s="8" t="s">
-        <v>116</v>
+      <c r="A36" t="s">
+        <v>158</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30">
+      <c r="A37" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D37" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="75">
+      <c r="A38" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="30">
-      <c r="A37" t="s">
-        <v>166</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" t="s">
-        <v>45</v>
-      </c>
-      <c r="G37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37"/>
-      <c r="I37" t="s">
-        <v>118</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="30">
-      <c r="A38" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38"/>
-      <c r="I38" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>121</v>
+      <c r="F38" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I38" t="s">
+        <v>170</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30">
       <c r="A39" s="8" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" t="s">
         <v>38</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="G39" s="8"/>
-      <c r="H39" s="9" t="s">
-        <v>104</v>
+      <c r="H39" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="I39" t="s">
-        <v>66</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K39" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K39" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="30">
-      <c r="A40" s="5" t="s">
-        <v>106</v>
+      <c r="A40" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="C40" t="s">
         <v>30</v>
@@ -2225,295 +2207,146 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
       </c>
       <c r="H40"/>
       <c r="I40" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>12</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30">
       <c r="A41" s="8" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>32</v>
+      </c>
+      <c r="G41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41"/>
+      <c r="I41" t="s">
+        <v>177</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30">
+      <c r="A42" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D42" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E42" t="s">
         <v>49</v>
       </c>
-      <c r="F41" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H41"/>
-      <c r="I41" s="8" t="s">
+      <c r="F42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42"/>
+      <c r="I42" t="s">
+        <v>177</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+      <c r="H43"/>
+      <c r="J43" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="75">
-      <c r="A42" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" t="s">
-        <v>129</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="I42" t="s">
-        <v>180</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="30">
-      <c r="A43" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44"/>
+      <c r="J44" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="8"/>
-      <c r="H43" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="I43" t="s">
-        <v>181</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="30">
-      <c r="A44" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" t="s">
-        <v>85</v>
-      </c>
-      <c r="G44" t="s">
-        <v>33</v>
-      </c>
-      <c r="H44"/>
-      <c r="I44" t="s">
-        <v>190</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="30">
-      <c r="A45" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
       <c r="D45" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" t="s">
-        <v>25</v>
-      </c>
-      <c r="F45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" t="s">
-        <v>33</v>
-      </c>
-      <c r="H45"/>
-      <c r="I45" t="s">
-        <v>190</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="30">
-      <c r="A46" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" t="s">
-        <v>172</v>
-      </c>
-      <c r="G46" t="s">
-        <v>33</v>
-      </c>
-      <c r="H46"/>
-      <c r="I46" t="s">
-        <v>190</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="30">
-      <c r="A47" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
-        <v>38</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E47" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F47" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H47"/>
-      <c r="I47" t="s">
-        <v>190</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48"/>
-      <c r="J48" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" t="s">
-        <v>49</v>
-      </c>
-      <c r="H49"/>
-      <c r="J49" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="A50" t="s">
-        <v>137</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F50" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8" t="s">
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J50" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="K50" s="8"/>
+      <c r="J45" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed failed validitions from Notify excel
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="187">
   <si>
     <t>API</t>
   </si>
@@ -121,9 +121,6 @@
     <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
   </si>
   <si>
-    <t>comments.id</t>
-  </si>
-  <si>
     <t>OPQA-208</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
     <t>Verify that user is able to add comments on the posts.</t>
   </si>
   <si>
-    <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Notification Test"}</t>
-  </si>
-  <si>
     <t>OPQA-215</t>
   </si>
   <si>
@@ -364,12 +358,6 @@
     <t>status=200||hasAppreciated=UP||targetType=posts||appreciateCount=2||targetId=(OPQA-360_id)</t>
   </si>
   <si>
-    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||comment.id=(OPQA-385_comments.id)||comment.text=Notification Test</t>
-  </si>
-  <si>
-    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||comment.id=(OPQA-236_comments.id)||comment.text=Notification Test</t>
-  </si>
-  <si>
     <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||publication.id=(OPQA-360_id)||publication.title=Creating Post For API Notification Testing</t>
   </si>
   <si>
@@ -502,12 +490,6 @@
     <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
   </si>
   <si>
-    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER4)||comments.data.text=Notification Test||publication.id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER4)||comment.text=Notification Test||publication.id=(OPQA-360_id)</t>
-  </si>
-  <si>
     <t>OPQA-1431||OPQA-310_2</t>
   </si>
   <si>
@@ -521,9 +503,6 @@
   </si>
   <si>
     <t>status=200||type=watchlist||ispublic=true</t>
-  </si>
-  <si>
-    <t>status=200||type=PUBLIC_WATCHLIST||issuer.truid=(SYS_USER3)||id=(OPQA-312_id)||publication.action=CREATE_WATCHLIST</t>
   </si>
   <si>
     <t>id||name</t>
@@ -547,9 +526,6 @@
   </si>
   <si>
     <t>{"name":"Public watchList for Notification testing","desc":"Creating public watchList for Notification testing","ispublic":true,"type":"watchlist"}</t>
-  </si>
-  <si>
-    <t>status=200||type=PUBLIC_WATCHLIST||issuer.truid=(SYS_USER3)||id=(OPQA-312_id)||publication.action=EDIT_PERMISSIONS_IN_WATCHLIST</t>
   </si>
   <si>
     <t>/container/(OPQA-312_id)/items?type=watchlist</t>
@@ -573,9 +549,6 @@
     <t>hits.id</t>
   </si>
   <si>
-    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.id)","content":"Notification Test"}</t>
-  </si>
-  <si>
     <t>{
 "items":
 [{
@@ -585,9 +558,6 @@
 }</t>
   </si>
   <si>
-    <t>{"targetType":"wos","targetId":"(OPQA-874_hits.id)","content":"Notification Test"}</t>
-  </si>
-  <si>
     <t>{
 "items":
 [{
@@ -597,16 +567,43 @@
 }</t>
   </si>
   <si>
-    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-874_hits.id)</t>
-  </si>
-  <si>
-    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-898_hits.id)</t>
-  </si>
-  <si>
-    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=Notification Test||publication.id=(OPQA-898_hits.id)</t>
-  </si>
-  <si>
-    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=Notification Test||publication.id=(OPQA-874_hits.id)</t>
+    <t>{"targetType":"wos","targetId":"(OPQA-874_hits.id)","content":"Notification Test(ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>comments.id||comments.content</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=(OPQA-236_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=(OPQA-236_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER4)||comments.data.text=(OPQA-385_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER4)||comment.text=(OPQA-385_comments.content)</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_id)","content":"Notification Test(ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"patents","targetId":"(OPQA-898_hits.id)","content":"Notification Test(ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||comment.id=(OPQA-385_comments.id)||comment.text=(OPQA-385_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=WatchedDocumentComment||comments.data.issuer.truid=(SYS_USER2)||comments.data.text=(OPQA-1431_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=DocumentComment||comment.issuer.truid=(SYS_USER2)||comment.text=(OPQA-1431_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=Appreciation||profiles.truid=(SYS_USER3)||profiles.truid=(SYS_USER1)||comment.id=(OPQA-236_comments.id)||comment.text=(OPQA-236_comments.content)</t>
+  </si>
+  <si>
+    <t>status=200||type=PUBLIC_WATCHLIST||issuer.truid=(SYS_USER3)</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1005,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L49"/>
+      <selection activeCell="L2" sqref="L2:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1023,7 +1020,7 @@
     <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="93.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1124,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>18</v>
@@ -1142,48 +1139,48 @@
         <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1193,16 +1190,16 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
@@ -1214,31 +1211,31 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>26</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -1247,16 +1244,16 @@
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
       <c r="J8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -1275,49 +1272,49 @@
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -1329,44 +1326,44 @@
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
         <v>26</v>
       </c>
       <c r="H11"/>
       <c r="I11" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>12</v>
@@ -1375,29 +1372,29 @@
     </row>
     <row r="13" spans="1:12" ht="75">
       <c r="A13" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>12</v>
@@ -1406,10 +1403,10 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -1421,43 +1418,43 @@
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
         <v>26</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="105">
       <c r="A15" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>12</v>
@@ -1465,16 +1462,16 @@
     </row>
     <row r="16" spans="1:12" ht="150">
       <c r="A16" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>13</v>
@@ -1484,22 +1481,22 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -1518,18 +1515,18 @@
       </c>
       <c r="H17"/>
       <c r="I17" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
@@ -1541,31 +1538,31 @@
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G18" t="s">
         <v>26</v>
       </c>
       <c r="H18"/>
       <c r="I18" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>13</v>
@@ -1575,53 +1572,53 @@
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -1633,25 +1630,25 @@
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
         <v>26</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="45">
       <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -1667,24 +1664,24 @@
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="4" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I22" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>34</v>
+        <v>74</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -1696,25 +1693,25 @@
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G23" t="s">
         <v>26</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1736,21 +1733,21 @@
         <v>30</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1759,50 +1756,50 @@
         <v>33</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I25" t="s">
         <v>30</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I26" t="s">
         <v>30</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -1814,34 +1811,34 @@
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
         <v>26</v>
       </c>
       <c r="H27"/>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>116</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30">
       <c r="A28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C28" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
         <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>41</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>14</v>
@@ -1851,33 +1848,33 @@
         <v>30</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="105">
       <c r="A29" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I29" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>12</v>
@@ -1885,10 +1882,10 @@
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>31</v>
@@ -1900,28 +1897,28 @@
         <v>13</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="9" t="s">
-        <v>93</v>
+        <v>180</v>
       </c>
       <c r="I30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>34</v>
+        <v>156</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1933,25 +1930,25 @@
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G31" t="s">
         <v>26</v>
       </c>
       <c r="H31"/>
       <c r="I31" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1970,18 +1967,18 @@
       </c>
       <c r="H32"/>
       <c r="I32" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1993,14 +1990,14 @@
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" t="s">
         <v>26</v>
       </c>
       <c r="H33"/>
       <c r="I33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>12</v>
@@ -2008,16 +2005,16 @@
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>13</v>
@@ -2027,51 +2024,51 @@
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30">
       <c r="A36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
@@ -2083,81 +2080,81 @@
         <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G36" t="s">
         <v>26</v>
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30">
       <c r="A37" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="105">
       <c r="A38" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I38" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="30">
+    <row r="39" spans="1:11" ht="45">
       <c r="A39" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
@@ -2173,24 +2170,24 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>34</v>
+        <v>74</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="30">
       <c r="A40" s="8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
@@ -2202,25 +2199,25 @@
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G40" t="s">
         <v>26</v>
       </c>
       <c r="H40"/>
       <c r="I40" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30">
       <c r="A41" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -2239,107 +2236,107 @@
       </c>
       <c r="H41"/>
       <c r="I41" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30">
       <c r="A42" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
         <v>31</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H42"/>
       <c r="I42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H43"/>
       <c r="J43" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H44"/>
       <c r="J44" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K45" s="8"/>
     </row>

</xml_diff>

<commit_message>
Modified 1PNotify service into 1PNotifyV1 in NotifyTestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/test-data/NotifyTestData.xlsx
+++ b/src/test/test-data/NotifyTestData.xlsx
@@ -88,9 +88,6 @@
     <t>Verify that to get notification for user</t>
   </si>
   <si>
-    <t>1PNOTIFY</t>
-  </si>
-  <si>
     <t>/notify/list</t>
   </si>
   <si>
@@ -604,6 +601,9 @@
   </si>
   <si>
     <t>status=200||type=PUBLIC_WATCHLIST||issuer.truid=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>1PNOTIFYV1</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1005,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L59"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1070,19 +1070,19 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>26</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="5" t="s">
@@ -1091,26 +1091,26 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1121,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>18</v>
@@ -1139,48 +1139,48 @@
         <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1190,52 +1190,52 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -1244,126 +1244,126 @@
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
       <c r="J8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E9" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
         <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
       </c>
       <c r="H9"/>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E11" t="s">
         <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11"/>
       <c r="I11" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75">
       <c r="A12" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>12</v>
@@ -1372,29 +1372,29 @@
     </row>
     <row r="13" spans="1:12" ht="75">
       <c r="A13" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>12</v>
@@ -1403,58 +1403,58 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="105">
       <c r="A15" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>12</v>
@@ -1462,16 +1462,16 @@
     </row>
     <row r="16" spans="1:12" ht="150">
       <c r="A16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>13</v>
@@ -1481,180 +1481,180 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="C17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E17" t="s">
         <v>19</v>
       </c>
       <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
         <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
       </c>
       <c r="H17"/>
       <c r="I17" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="C18" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18"/>
       <c r="I18" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="C21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E21" t="s">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21"/>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
       <c r="A22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>13</v>
@@ -1664,217 +1664,217 @@
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I22" t="s">
         <v>15</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30">
       <c r="A23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H23"/>
       <c r="I23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="30">
       <c r="A24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
       </c>
       <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="s">
         <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>26</v>
       </c>
       <c r="H24"/>
       <c r="I24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="30">
       <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="30">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="30">
       <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="C27" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H27"/>
       <c r="I27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30">
       <c r="A28" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="6" t="s">
+      <c r="E28" t="s">
         <v>39</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H28"/>
       <c r="I28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="105">
       <c r="A29" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F29" t="s">
+        <v>167</v>
+      </c>
+      <c r="H29" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="I29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J29" s="5" t="s">
         <v>12</v>
@@ -1882,122 +1882,122 @@
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>91</v>
-      </c>
       <c r="C30" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="C31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E31" t="s">
         <v>19</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H31"/>
       <c r="I31" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="30">
       <c r="A32" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" t="s">
         <v>25</v>
-      </c>
-      <c r="G32" t="s">
-        <v>26</v>
       </c>
       <c r="H32"/>
       <c r="I32" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="30">
       <c r="A33" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="C33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H33"/>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>12</v>
@@ -2005,145 +2005,145 @@
     </row>
     <row r="34" spans="1:11" ht="30">
       <c r="A34" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>99</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="30">
       <c r="A35" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="30">
       <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>133</v>
-      </c>
       <c r="C36" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H36"/>
       <c r="I36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="30">
       <c r="A37" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="105">
       <c r="A38" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>12</v>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="39" spans="1:11" ht="45">
       <c r="A39" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>13</v>
@@ -2170,173 +2170,173 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K39" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="30">
       <c r="A40" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
+        <v>186</v>
+      </c>
+      <c r="D40" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E40" t="s">
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H40"/>
       <c r="I40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="30">
       <c r="A41" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C41" t="s">
+        <v>186</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E41" t="s">
         <v>19</v>
       </c>
       <c r="F41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
         <v>25</v>
-      </c>
-      <c r="G41" t="s">
-        <v>26</v>
       </c>
       <c r="H41"/>
       <c r="I41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="30">
       <c r="A42" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>14</v>
       </c>
       <c r="H42"/>
       <c r="I42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H43"/>
       <c r="J43" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H44"/>
       <c r="J44" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="E45" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K45" s="8"/>
     </row>

</xml_diff>